<commit_message>
add urlencode write file
add urlencode write file
</commit_message>
<xml_diff>
--- a/doc/在线编译需求.xlsx
+++ b/doc/在线编译需求.xlsx
@@ -22,79 +22,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>把</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>HTTP</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>的每一部分都能提取出来，包括：请求头、消息头，消息体，</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>Get</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>提交的内容，</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>Post</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>提交的内容</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>截止时间</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -245,6 +172,79 @@
   </si>
   <si>
     <t>使用工厂模式进行重构</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>把</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>HTTP</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>的每一部分都能提取出来，包括：请求头、消息头，消息体，</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Get</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>提交的内容，</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Post</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>提交的内容</t>
+    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -707,7 +707,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -720,7 +720,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="23.25">
       <c r="A1" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -729,16 +729,16 @@
     <row r="2" spans="1:5" ht="22.5">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="42.75">
@@ -746,16 +746,16 @@
         <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="D3" s="7">
         <v>42170</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="85.5">
@@ -763,10 +763,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D4" s="7">
         <v>42172</v>
@@ -778,10 +778,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="9" t="s">
         <v>4</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>5</v>
       </c>
       <c r="D5" s="7">
         <v>42174</v>
@@ -793,10 +793,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D6" s="10"/>
       <c r="E6" s="6"/>
@@ -806,7 +806,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C7" s="11"/>
       <c r="D7" s="10"/>
@@ -817,7 +817,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8" s="11"/>
       <c r="D8" s="10"/>
@@ -828,7 +828,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C9" s="11"/>
       <c r="D9" s="10"/>
@@ -839,7 +839,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C10" s="11"/>
       <c r="D10" s="10"/>
@@ -847,7 +847,7 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>